<commit_message>
feat: buscar departamento por desc y estado. Paginar resultados.
</commit_message>
<xml_diff>
--- a/doc/pdf/usoSesion.xlsx
+++ b/doc/pdf/usoSesion.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">USO DE LA SESIÓN - $_SESSION – EN LA APLICACIÓN</t>
   </si>
@@ -280,7 +280,133 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Objeto que guarda el codigo del departamento seleccionado desde la ventana vMtoDepartamentos.</t>
+    <t xml:space="preserve">Texto que guarda el codigo del departamento seleccionado desde la ventana vMtoDepartamentos.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$_SESSION [</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">descDepartamentoBuscadaEnCurso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Texto que guarda la descripcion introducida en el campo de busqueda de la v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">MtoDepartamentos.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$_SESSION [</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">estadoDepartamentoBuscadoEnCurso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Texto que guarda el estado seleccionado en los radio buton de la vMtoDepartamentos. (alta/baja/todos)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$_SESSION [</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">paginaActualTablaDepartamentos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Texto que guarda el número de página actual de la tabla que muestra los departamentos en la vMtoDepartamentos.</t>
   </si>
 </sst>
 </file>
@@ -290,7 +416,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,6 +462,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -400,7 +532,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -430,6 +562,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -682,16 +818,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:C11"/>
+  <dimension ref="B2:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="63.85"/>
   </cols>
   <sheetData>
@@ -717,7 +853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
@@ -725,7 +861,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -733,7 +869,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
@@ -749,7 +885,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="44.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
@@ -757,7 +893,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="31.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -765,6 +901,31 @@
         <v>16</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="31.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="31.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="30.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>

</xml_diff>

<commit_message>
feat: Añadir cambiar contraseña en vMtoUsuarios
</commit_message>
<xml_diff>
--- a/doc/pdf/usoSesion.xlsx
+++ b/doc/pdf/usoSesion.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">USO DE LA SESIÓN - $_SESSION – EN LA APLICACIÓN</t>
   </si>
@@ -316,25 +316,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Texto que guarda la descripcion introducida en el campo de busqueda de la v</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">MtoDepartamentos.</t>
-    </r>
+    <t xml:space="preserve">Texto que guarda la descripcion introducida en el campo de busqueda de la vMtoDepartamentos.</t>
   </si>
   <si>
     <r>
@@ -407,6 +389,42 @@
   </si>
   <si>
     <t xml:space="preserve">Texto que guarda el número de página actual de la tabla que muestra los departamentos en la vMtoDepartamentos.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$_SESSION [</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">codDepartamentoEnCursoRest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Texto que guarda el codigo del departamento seleccionado desde la ventana Rest para su uso en la Mi Api.</t>
   </si>
 </sst>
 </file>
@@ -821,7 +839,7 @@
   <dimension ref="B2:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -913,7 +931,7 @@
       <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -921,8 +939,16 @@
       <c r="B14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="5" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>